<commit_message>
Excels update Jna 25
</commit_message>
<xml_diff>
--- a/src/assets/Excells/CotisationSpeciale0.xlsx
+++ b/src/assets/Excells/CotisationSpeciale0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bwamutalamiantezila/Documents/LukalaPhoto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7DE54C-B95F-E742-A738-BFF9FA406C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668F449A-0714-D84B-B912-88477CC514E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2300" windowWidth="30240" windowHeight="16500" xr2:uid="{68E375EF-7E04-A04A-8B5D-972BEA3F72AD}"/>
+    <workbookView xWindow="1140" yWindow="8160" windowWidth="35900" windowHeight="16600" xr2:uid="{68E375EF-7E04-A04A-8B5D-972BEA3F72AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="74">
   <si>
     <t>Eugenie Malayi</t>
   </si>
@@ -249,6 +249,15 @@
   </si>
   <si>
     <t>Février</t>
+  </si>
+  <si>
+    <t>Ntwa Nzeze</t>
+  </si>
+  <si>
+    <t>DENZOU Mvula</t>
+  </si>
+  <si>
+    <t>René Mamingi</t>
   </si>
 </sst>
 </file>
@@ -420,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -543,6 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF6F12D5-1178-994A-98D1-482C6B1D858E}">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,11 +906,12 @@
     <col min="9" max="9" width="13.5" style="23" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" style="23" customWidth="1"/>
     <col min="11" max="11" width="15" style="23" customWidth="1"/>
-    <col min="12" max="18" width="13.1640625" style="23" customWidth="1"/>
-    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+    <col min="12" max="19" width="13.1640625" style="23" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="28" customFormat="1" ht="77" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="28" customFormat="1" ht="77" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
@@ -955,9 +966,12 @@
       <c r="R1" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="38"/>
-    </row>
-    <row r="2" spans="1:19" s="28" customFormat="1" ht="31" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S1" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="38"/>
+    </row>
+    <row r="2" spans="1:21" s="28" customFormat="1" ht="31" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="45" t="s">
@@ -1002,9 +1016,12 @@
       <c r="R2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="39"/>
-    </row>
-    <row r="3" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="39"/>
+    </row>
+    <row r="3" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1031,35 +1048,38 @@
         <v>10</v>
       </c>
       <c r="J3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R3" s="9">
-        <v>0</v>
-      </c>
-      <c r="S3" s="40"/>
-    </row>
-    <row r="4" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="S3" s="9">
+        <v>0</v>
+      </c>
+      <c r="T3" s="40"/>
+    </row>
+    <row r="4" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -1089,32 +1109,35 @@
         <v>10</v>
       </c>
       <c r="K4" s="34">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L4" s="34">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R4" s="9">
-        <v>0</v>
-      </c>
-      <c r="S4" s="40"/>
-    </row>
-    <row r="5" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="S4" s="9">
+        <v>0</v>
+      </c>
+      <c r="T4" s="40"/>
+    </row>
+    <row r="5" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
@@ -1165,11 +1188,14 @@
         <v>10</v>
       </c>
       <c r="R5" s="9">
-        <v>0</v>
-      </c>
-      <c r="S5" s="40"/>
-    </row>
-    <row r="6" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="S5" s="9">
+        <v>10</v>
+      </c>
+      <c r="T5" s="40"/>
+    </row>
+    <row r="6" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1222,9 +1248,12 @@
       <c r="R6" s="9">
         <v>0</v>
       </c>
-      <c r="S6" s="40"/>
-    </row>
-    <row r="7" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S6" s="9">
+        <v>0</v>
+      </c>
+      <c r="T6" s="40"/>
+    </row>
+    <row r="7" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1254,32 +1283,35 @@
         <v>10</v>
       </c>
       <c r="K7" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L7" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M7" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N7" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O7" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P7" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R7" s="9">
-        <v>0</v>
-      </c>
-      <c r="S7" s="40"/>
-    </row>
-    <row r="8" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="S7" s="9">
+        <v>0</v>
+      </c>
+      <c r="T7" s="40"/>
+    </row>
+    <row r="8" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
@@ -1332,9 +1364,12 @@
       <c r="R8" s="9">
         <v>0</v>
       </c>
-      <c r="S8" s="40"/>
-    </row>
-    <row r="9" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S8" s="9">
+        <v>0</v>
+      </c>
+      <c r="T8" s="40"/>
+    </row>
+    <row r="9" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>21</v>
       </c>
@@ -1387,9 +1422,12 @@
       <c r="R9" s="9">
         <v>0</v>
       </c>
-      <c r="S9" s="40"/>
-    </row>
-    <row r="10" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S9" s="9">
+        <v>0</v>
+      </c>
+      <c r="T9" s="40"/>
+    </row>
+    <row r="10" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
@@ -1406,35 +1444,35 @@
         <v>50</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>14</v>
+      <c r="G10" s="9">
+        <v>10</v>
+      </c>
+      <c r="H10" s="9">
+        <v>10</v>
+      </c>
+      <c r="I10" s="9">
+        <v>10</v>
+      </c>
+      <c r="J10" s="9">
+        <v>10</v>
       </c>
       <c r="K10" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L10" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M10" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N10" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O10" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P10" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q10" s="9">
         <v>0</v>
@@ -1442,9 +1480,12 @@
       <c r="R10" s="9">
         <v>0</v>
       </c>
-      <c r="S10" s="40"/>
-    </row>
-    <row r="11" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S10" s="9">
+        <v>0</v>
+      </c>
+      <c r="T10" s="40"/>
+    </row>
+    <row r="11" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>39</v>
       </c>
@@ -1497,9 +1538,12 @@
       <c r="R11" s="9">
         <v>0</v>
       </c>
-      <c r="S11" s="40"/>
-    </row>
-    <row r="12" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S11" s="9">
+        <v>0</v>
+      </c>
+      <c r="T11" s="40"/>
+    </row>
+    <row r="12" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>60</v>
       </c>
@@ -1552,9 +1596,12 @@
       <c r="R12" s="9">
         <v>0</v>
       </c>
-      <c r="S12" s="40"/>
-    </row>
-    <row r="13" spans="1:19" s="3" customFormat="1" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S12" s="9">
+        <v>0</v>
+      </c>
+      <c r="T12" s="40"/>
+    </row>
+    <row r="13" spans="1:21" s="3" customFormat="1" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
@@ -1571,62 +1618,67 @@
         <v>450</v>
       </c>
       <c r="F13" s="36">
-        <v>-51.5</v>
+        <v>-210</v>
       </c>
       <c r="G13" s="29">
         <f>SUM(G3:G12)</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H13" s="29">
         <f>0+SUM(H3:H12)</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I13" s="29">
         <f>SUM(I3:I12)</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J13" s="29">
         <f>SUM(J3:J12)</f>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K13" s="29">
         <f>SUM(K3:K12)</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="L13" s="29">
         <f>SUM(L3:L12)</f>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="M13" s="29">
         <f t="shared" ref="M13:R13" si="0">SUM(M3:M12)</f>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="N13" s="29">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="O13" s="29">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="P13" s="29">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="Q13" s="29">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="R13" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S13" s="42">
-        <f>SUM(D13:L13)</f>
-        <v>878.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="S13" s="29">
+        <f>SUM(S3:S12)</f>
+        <v>10</v>
+      </c>
+      <c r="T13" s="42">
+        <f>SUM(D13:S13)</f>
+        <v>1140</v>
+      </c>
+      <c r="U13" s="48"/>
+    </row>
+    <row r="14" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
       <c r="B14" s="14"/>
       <c r="C14" s="8"/>
@@ -1673,9 +1725,12 @@
       <c r="R14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="S14" s="40"/>
-    </row>
-    <row r="15" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T14" s="40"/>
+    </row>
+    <row r="15" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="14"/>
       <c r="C15" s="8"/>
@@ -1722,9 +1777,12 @@
       <c r="R15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="S15" s="40"/>
-    </row>
-    <row r="16" spans="1:19" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T15" s="40"/>
+    </row>
+    <row r="16" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="14"/>
       <c r="C16" s="45" t="s">
@@ -1769,9 +1827,12 @@
       <c r="R16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="S16" s="40"/>
-    </row>
-    <row r="17" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T16" s="40"/>
+    </row>
+    <row r="17" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>4</v>
       </c>
@@ -1824,10 +1885,13 @@
       <c r="R17" s="44">
         <v>0</v>
       </c>
-      <c r="S17" s="40"/>
-      <c r="U17" s="6"/>
-    </row>
-    <row r="18" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S17" s="44">
+        <v>0</v>
+      </c>
+      <c r="T17" s="40"/>
+      <c r="V17" s="6"/>
+    </row>
+    <row r="18" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
@@ -1880,10 +1944,13 @@
       <c r="R18" s="44">
         <v>0</v>
       </c>
-      <c r="S18" s="40"/>
-      <c r="U18" s="6"/>
-    </row>
-    <row r="19" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S18" s="44">
+        <v>0</v>
+      </c>
+      <c r="T18" s="40"/>
+      <c r="V18" s="6"/>
+    </row>
+    <row r="19" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
@@ -1936,10 +2003,13 @@
       <c r="R19" s="44">
         <v>0</v>
       </c>
-      <c r="S19" s="40"/>
-      <c r="U19" s="6"/>
-    </row>
-    <row r="20" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S19" s="44">
+        <v>0</v>
+      </c>
+      <c r="T19" s="40"/>
+      <c r="V19" s="6"/>
+    </row>
+    <row r="20" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
@@ -1956,35 +2026,35 @@
         <v>50</v>
       </c>
       <c r="F20" s="16"/>
-      <c r="G20" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>14</v>
+      <c r="G20" s="16">
+        <v>10</v>
+      </c>
+      <c r="H20" s="16">
+        <v>10</v>
+      </c>
+      <c r="I20" s="16">
+        <v>10</v>
+      </c>
+      <c r="J20" s="16">
+        <v>10</v>
       </c>
       <c r="K20" s="16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L20" s="16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M20" s="44">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N20" s="44">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O20" s="44">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P20" s="44">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q20" s="44">
         <v>0</v>
@@ -1992,10 +2062,13 @@
       <c r="R20" s="44">
         <v>0</v>
       </c>
-      <c r="S20" s="40"/>
-      <c r="U20" s="6"/>
-    </row>
-    <row r="21" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S20" s="44">
+        <v>0</v>
+      </c>
+      <c r="T20" s="40"/>
+      <c r="V20" s="6"/>
+    </row>
+    <row r="21" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>29</v>
       </c>
@@ -2009,7 +2082,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="16">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16" t="s">
@@ -2048,10 +2121,13 @@
       <c r="R21" s="44">
         <v>0</v>
       </c>
-      <c r="S21" s="40"/>
-      <c r="U21" s="6"/>
-    </row>
-    <row r="22" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S21" s="44">
+        <v>0</v>
+      </c>
+      <c r="T21" s="40"/>
+      <c r="V21" s="6"/>
+    </row>
+    <row r="22" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
@@ -2104,10 +2180,13 @@
       <c r="R22" s="44">
         <v>0</v>
       </c>
-      <c r="S22" s="40"/>
-      <c r="U22" s="6"/>
-    </row>
-    <row r="23" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S22" s="44">
+        <v>0</v>
+      </c>
+      <c r="T22" s="40"/>
+      <c r="V22" s="6"/>
+    </row>
+    <row r="23" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>28</v>
       </c>
@@ -2160,10 +2239,13 @@
       <c r="R23" s="44">
         <v>0</v>
       </c>
-      <c r="S23" s="40"/>
-      <c r="U23" s="6"/>
-    </row>
-    <row r="24" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S23" s="44">
+        <v>0</v>
+      </c>
+      <c r="T23" s="40"/>
+      <c r="V23" s="6"/>
+    </row>
+    <row r="24" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>47</v>
       </c>
@@ -2216,10 +2298,13 @@
       <c r="R24" s="44">
         <v>0</v>
       </c>
-      <c r="S24" s="40"/>
-      <c r="U24" s="6"/>
-    </row>
-    <row r="25" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S24" s="44">
+        <v>0</v>
+      </c>
+      <c r="T24" s="40"/>
+      <c r="V24" s="6"/>
+    </row>
+    <row r="25" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>27</v>
       </c>
@@ -2272,10 +2357,13 @@
       <c r="R25" s="44">
         <v>0</v>
       </c>
-      <c r="S25" s="40"/>
-      <c r="U25" s="6"/>
-    </row>
-    <row r="26" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S25" s="44">
+        <v>0</v>
+      </c>
+      <c r="T25" s="40"/>
+      <c r="V25" s="6"/>
+    </row>
+    <row r="26" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -2328,10 +2416,13 @@
       <c r="R26" s="44">
         <v>0</v>
       </c>
-      <c r="S26" s="40"/>
-      <c r="U26" s="6"/>
-    </row>
-    <row r="27" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S26" s="44">
+        <v>0</v>
+      </c>
+      <c r="T26" s="40"/>
+      <c r="V26" s="6"/>
+    </row>
+    <row r="27" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>22</v>
       </c>
@@ -2384,10 +2475,13 @@
       <c r="R27" s="44">
         <v>0</v>
       </c>
-      <c r="S27" s="40"/>
-      <c r="U27" s="6"/>
-    </row>
-    <row r="28" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S27" s="44">
+        <v>0</v>
+      </c>
+      <c r="T27" s="40"/>
+      <c r="V27" s="6"/>
+    </row>
+    <row r="28" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>35</v>
       </c>
@@ -2440,10 +2534,13 @@
       <c r="R28" s="16">
         <v>10</v>
       </c>
-      <c r="S28" s="40"/>
-      <c r="U28" s="6"/>
-    </row>
-    <row r="29" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S28" s="16">
+        <v>0</v>
+      </c>
+      <c r="T28" s="40"/>
+      <c r="V28" s="6"/>
+    </row>
+    <row r="29" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>23</v>
       </c>
@@ -2496,10 +2593,13 @@
       <c r="R29" s="44">
         <v>0</v>
       </c>
-      <c r="S29" s="40"/>
-      <c r="U29" s="6"/>
-    </row>
-    <row r="30" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S29" s="44">
+        <v>0</v>
+      </c>
+      <c r="T29" s="40"/>
+      <c r="V29" s="6"/>
+    </row>
+    <row r="30" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>6</v>
       </c>
@@ -2552,10 +2652,13 @@
       <c r="R30" s="44">
         <v>0</v>
       </c>
-      <c r="S30" s="40"/>
-      <c r="U30" s="6"/>
-    </row>
-    <row r="31" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S30" s="44">
+        <v>0</v>
+      </c>
+      <c r="T30" s="40"/>
+      <c r="V30" s="6"/>
+    </row>
+    <row r="31" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>33</v>
       </c>
@@ -2569,7 +2672,7 @@
         <v>10</v>
       </c>
       <c r="E31" s="16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="16" t="s">
@@ -2608,10 +2711,13 @@
       <c r="R31" s="44">
         <v>0</v>
       </c>
-      <c r="S31" s="40"/>
-      <c r="U31" s="6"/>
-    </row>
-    <row r="32" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S31" s="44">
+        <v>0</v>
+      </c>
+      <c r="T31" s="40"/>
+      <c r="V31" s="6"/>
+    </row>
+    <row r="32" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>11</v>
       </c>
@@ -2664,10 +2770,13 @@
       <c r="R32" s="44">
         <v>0</v>
       </c>
-      <c r="S32" s="40"/>
-      <c r="U32" s="6"/>
-    </row>
-    <row r="33" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S32" s="44">
+        <v>0</v>
+      </c>
+      <c r="T32" s="40"/>
+      <c r="V32" s="6"/>
+    </row>
+    <row r="33" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>36</v>
       </c>
@@ -2720,10 +2829,13 @@
       <c r="R33" s="44">
         <v>0</v>
       </c>
-      <c r="S33" s="40"/>
-      <c r="U33" s="6"/>
-    </row>
-    <row r="34" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S33" s="44">
+        <v>0</v>
+      </c>
+      <c r="T33" s="40"/>
+      <c r="V33" s="6"/>
+    </row>
+    <row r="34" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>31</v>
       </c>
@@ -2740,14 +2852,14 @@
         <v>0</v>
       </c>
       <c r="F34" s="16"/>
-      <c r="G34" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>14</v>
+      <c r="G34" s="16">
+        <v>10</v>
+      </c>
+      <c r="H34" s="16">
+        <v>10</v>
+      </c>
+      <c r="I34" s="16">
+        <v>10</v>
       </c>
       <c r="J34" s="16" t="s">
         <v>14</v>
@@ -2776,24 +2888,25 @@
       <c r="R34" s="44">
         <v>0</v>
       </c>
-      <c r="S34" s="40"/>
-      <c r="U34" s="6"/>
-    </row>
-    <row r="35" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S34" s="44">
+        <v>0</v>
+      </c>
+      <c r="T34" s="40"/>
+      <c r="V34" s="6"/>
+    </row>
+    <row r="35" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="C35" s="8"/>
       <c r="D35" s="16">
         <v>10</v>
       </c>
       <c r="E35" s="16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F35" s="16"/>
       <c r="G35" s="16">
@@ -2832,74 +2945,78 @@
       <c r="R35" s="44">
         <v>0</v>
       </c>
-      <c r="S35" s="40"/>
-      <c r="U35" s="6"/>
-    </row>
-    <row r="36" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S35" s="44">
+        <v>0</v>
+      </c>
+      <c r="T35" s="40"/>
+      <c r="V35" s="6"/>
+    </row>
+    <row r="36" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C36" s="8"/>
       <c r="D36" s="16">
         <v>10</v>
       </c>
       <c r="E36" s="16">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F36" s="16"/>
       <c r="G36" s="16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H36" s="16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I36" s="16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J36" s="16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K36" s="16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L36" s="16">
         <v>0</v>
       </c>
-      <c r="M36" s="44">
-        <v>0</v>
-      </c>
-      <c r="N36" s="44">
-        <v>0</v>
-      </c>
-      <c r="O36" s="44">
-        <v>0</v>
-      </c>
-      <c r="P36" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="44">
-        <v>0</v>
-      </c>
-      <c r="R36" s="44">
-        <v>0</v>
-      </c>
-      <c r="S36" s="40"/>
-      <c r="U36" s="6"/>
-    </row>
-    <row r="37" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M36" s="16">
+        <v>0</v>
+      </c>
+      <c r="N36" s="16">
+        <v>0</v>
+      </c>
+      <c r="O36" s="16">
+        <v>0</v>
+      </c>
+      <c r="P36" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="16">
+        <v>0</v>
+      </c>
+      <c r="R36" s="16">
+        <v>0</v>
+      </c>
+      <c r="S36" s="16">
+        <v>0</v>
+      </c>
+      <c r="T36" s="40"/>
+      <c r="V36" s="6"/>
+    </row>
+    <row r="37" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="D37" s="16">
         <v>10</v>
@@ -2944,18 +3061,21 @@
       <c r="R37" s="44">
         <v>0</v>
       </c>
-      <c r="S37" s="40"/>
-      <c r="U37" s="6"/>
-    </row>
-    <row r="38" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S37" s="44">
+        <v>0</v>
+      </c>
+      <c r="T37" s="40"/>
+      <c r="V37" s="6"/>
+    </row>
+    <row r="38" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D38" s="16">
         <v>10</v>
@@ -3000,12 +3120,15 @@
       <c r="R38" s="44">
         <v>0</v>
       </c>
-      <c r="S38" s="40"/>
-      <c r="U38" s="6"/>
-    </row>
-    <row r="39" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S38" s="44">
+        <v>0</v>
+      </c>
+      <c r="T38" s="40"/>
+      <c r="V38" s="6"/>
+    </row>
+    <row r="39" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>13</v>
@@ -3056,31 +3179,40 @@
       <c r="R39" s="44">
         <v>0</v>
       </c>
-      <c r="S39" s="40"/>
-      <c r="U39" s="6"/>
-    </row>
-    <row r="40" spans="1:21" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="15" t="s">
-        <v>14</v>
+      <c r="S39" s="44">
+        <v>0</v>
+      </c>
+      <c r="T39" s="40"/>
+      <c r="V39" s="6"/>
+    </row>
+    <row r="40" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="16">
+        <v>10</v>
       </c>
       <c r="E40" s="16">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F40" s="16"/>
-      <c r="G40" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="16" t="s">
-        <v>14</v>
+      <c r="G40" s="16">
+        <v>0</v>
+      </c>
+      <c r="H40" s="16">
+        <v>0</v>
+      </c>
+      <c r="I40" s="16">
+        <v>0</v>
+      </c>
+      <c r="J40" s="16">
+        <v>0</v>
       </c>
       <c r="K40" s="16">
         <v>0</v>
@@ -3106,483 +3238,683 @@
       <c r="R40" s="44">
         <v>0</v>
       </c>
-      <c r="S40" s="40"/>
-    </row>
-    <row r="41" spans="1:21" s="2" customFormat="1" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="17">
-        <f>SUM(D17:D40)</f>
-        <v>220</v>
-      </c>
-      <c r="E41" s="17">
-        <f>SUM(E17:E40)</f>
-        <v>615</v>
-      </c>
-      <c r="F41" s="36">
-        <v>-390</v>
-      </c>
-      <c r="G41" s="30">
-        <f>SUM(H17:H40)</f>
-        <v>20</v>
-      </c>
-      <c r="H41" s="30">
-        <f>SUM(H17:H40)</f>
-        <v>20</v>
-      </c>
-      <c r="I41" s="30">
-        <f>SUM(I17:I40)</f>
-        <v>20</v>
-      </c>
-      <c r="J41" s="30">
-        <f>SUM(J17:J40)</f>
-        <v>10</v>
-      </c>
-      <c r="K41" s="30">
-        <f>SUM(K17:K40)</f>
-        <v>10</v>
-      </c>
-      <c r="L41" s="30">
-        <f>SUM(M17:M40)</f>
-        <v>10</v>
-      </c>
-      <c r="M41" s="30">
-        <f t="shared" ref="M41:R41" si="1">SUM(M17:M40)</f>
-        <v>10</v>
-      </c>
-      <c r="N41" s="30">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="O41" s="30">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="P41" s="30">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="Q41" s="30">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="R41" s="30">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="S41" s="43">
-        <f>SUM(D41:R41)</f>
-        <v>595</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" s="2" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
-      <c r="B42" s="14"/>
+      <c r="S40" s="44">
+        <v>0</v>
+      </c>
+      <c r="T40" s="40"/>
+      <c r="V40" s="6"/>
+    </row>
+    <row r="41" spans="1:22" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="16">
+        <v>10</v>
+      </c>
+      <c r="E41" s="16">
+        <v>50</v>
+      </c>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16">
+        <v>0</v>
+      </c>
+      <c r="H41" s="16">
+        <v>0</v>
+      </c>
+      <c r="I41" s="16">
+        <v>0</v>
+      </c>
+      <c r="J41" s="16">
+        <v>0</v>
+      </c>
+      <c r="K41" s="16">
+        <v>0</v>
+      </c>
+      <c r="L41" s="16">
+        <v>0</v>
+      </c>
+      <c r="M41" s="44">
+        <v>0</v>
+      </c>
+      <c r="N41" s="44">
+        <v>0</v>
+      </c>
+      <c r="O41" s="44">
+        <v>0</v>
+      </c>
+      <c r="P41" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="44">
+        <v>0</v>
+      </c>
+      <c r="R41" s="44">
+        <v>0</v>
+      </c>
+      <c r="S41" s="44">
+        <v>0</v>
+      </c>
+      <c r="T41" s="40"/>
+      <c r="V41" s="6"/>
+    </row>
+    <row r="42" spans="1:22" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="21">
-        <v>0</v>
-      </c>
-      <c r="F42" s="21"/>
-      <c r="G42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="M42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="N42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="O42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="P42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="R42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="S42" s="41"/>
-    </row>
-    <row r="43" spans="1:21" s="2" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="13"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" s="21">
-        <v>0</v>
-      </c>
-      <c r="F43" s="21"/>
-      <c r="G43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="M43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="N43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="O43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="P43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="R43" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="S43" s="41"/>
-    </row>
-    <row r="44" spans="1:21" s="2" customFormat="1" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E42" s="16">
+        <v>0</v>
+      </c>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K42" s="16">
+        <v>0</v>
+      </c>
+      <c r="L42" s="16">
+        <v>0</v>
+      </c>
+      <c r="M42" s="44">
+        <v>0</v>
+      </c>
+      <c r="N42" s="44">
+        <v>0</v>
+      </c>
+      <c r="O42" s="44">
+        <v>0</v>
+      </c>
+      <c r="P42" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="44">
+        <v>0</v>
+      </c>
+      <c r="R42" s="44">
+        <v>0</v>
+      </c>
+      <c r="S42" s="44">
+        <v>0</v>
+      </c>
+      <c r="T42" s="40"/>
+    </row>
+    <row r="43" spans="1:22" s="2" customFormat="1" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="17">
+        <f>SUM(D17:D42)</f>
+        <v>240</v>
+      </c>
+      <c r="E43" s="17">
+        <f>SUM(E17:E42)</f>
+        <v>650</v>
+      </c>
+      <c r="F43" s="36">
+        <v>-390</v>
+      </c>
+      <c r="G43" s="30">
+        <f>SUM(H17:H42)</f>
+        <v>50</v>
+      </c>
+      <c r="H43" s="30">
+        <f>SUM(H17:H42)</f>
+        <v>50</v>
+      </c>
+      <c r="I43" s="30">
+        <f>SUM(I17:I42)</f>
+        <v>50</v>
+      </c>
+      <c r="J43" s="30">
+        <f>SUM(J17:J42)</f>
+        <v>30</v>
+      </c>
+      <c r="K43" s="30">
+        <f>SUM(K17:K42)</f>
+        <v>30</v>
+      </c>
+      <c r="L43" s="30">
+        <f>SUM(M17:M42)</f>
+        <v>20</v>
+      </c>
+      <c r="M43" s="30">
+        <f t="shared" ref="M43:R43" si="1">SUM(M17:M42)</f>
+        <v>20</v>
+      </c>
+      <c r="N43" s="30">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="O43" s="30">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="P43" s="30">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="Q43" s="30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="R43" s="30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="S43" s="30">
+        <f>SUM(S17:S42)</f>
+        <v>0</v>
+      </c>
+      <c r="T43" s="43">
+        <f>SUM(D43:S43)</f>
+        <v>830</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" s="2" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="13"/>
       <c r="B44" s="14"/>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="8"/>
+      <c r="D44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="21">
+        <v>0</v>
+      </c>
+      <c r="F44" s="21"/>
+      <c r="G44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="R44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="S44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T44" s="41"/>
+    </row>
+    <row r="45" spans="1:22" s="2" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="21">
+        <v>0</v>
+      </c>
+      <c r="F45" s="21"/>
+      <c r="G45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="R45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="S45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T45" s="41"/>
+    </row>
+    <row r="46" spans="1:22" s="2" customFormat="1" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="13"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="46"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="M44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="N44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="O44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="P44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="R44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="S44" s="41"/>
-    </row>
-    <row r="45" spans="1:21" s="2" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="7" t="s">
+      <c r="D46" s="46"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="R46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="S46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T46" s="41"/>
+    </row>
+    <row r="47" spans="1:22" s="2" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B47" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="9">
-        <v>10</v>
-      </c>
-      <c r="E45" s="9">
+      <c r="D47" s="9">
+        <v>10</v>
+      </c>
+      <c r="E47" s="9">
         <v>100</v>
       </c>
-      <c r="F45" s="33"/>
-      <c r="G45" s="9">
-        <v>10</v>
-      </c>
-      <c r="H45" s="9">
-        <v>10</v>
-      </c>
-      <c r="I45" s="9">
-        <v>10</v>
-      </c>
-      <c r="J45" s="9">
-        <v>10</v>
-      </c>
-      <c r="K45" s="9">
-        <v>0</v>
-      </c>
-      <c r="L45" s="9">
-        <v>0</v>
-      </c>
-      <c r="M45" s="44">
-        <v>0</v>
-      </c>
-      <c r="N45" s="44">
-        <v>0</v>
-      </c>
-      <c r="O45" s="44">
-        <v>0</v>
-      </c>
-      <c r="P45" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="44">
-        <v>0</v>
-      </c>
-      <c r="R45" s="44">
-        <v>0</v>
-      </c>
-      <c r="S45" s="41"/>
-    </row>
-    <row r="46" spans="1:21" s="2" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="7" t="s">
+      <c r="F47" s="33"/>
+      <c r="G47" s="9">
+        <v>10</v>
+      </c>
+      <c r="H47" s="9">
+        <v>10</v>
+      </c>
+      <c r="I47" s="9">
+        <v>10</v>
+      </c>
+      <c r="J47" s="9">
+        <v>10</v>
+      </c>
+      <c r="K47" s="9">
+        <v>10</v>
+      </c>
+      <c r="L47" s="9">
+        <v>10</v>
+      </c>
+      <c r="M47" s="44">
+        <v>10</v>
+      </c>
+      <c r="N47" s="44">
+        <v>10</v>
+      </c>
+      <c r="O47" s="44">
+        <v>10</v>
+      </c>
+      <c r="P47" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q47" s="44">
+        <v>10</v>
+      </c>
+      <c r="R47" s="44">
+        <v>10</v>
+      </c>
+      <c r="S47" s="44">
+        <v>0</v>
+      </c>
+      <c r="T47" s="41"/>
+    </row>
+    <row r="48" spans="1:22" s="2" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="9">
+        <v>10</v>
+      </c>
+      <c r="E48" s="9">
+        <v>100</v>
+      </c>
+      <c r="F48" s="33"/>
+      <c r="G48" s="9">
+        <v>10</v>
+      </c>
+      <c r="H48" s="9">
+        <v>10</v>
+      </c>
+      <c r="I48" s="9">
+        <v>10</v>
+      </c>
+      <c r="J48" s="9">
+        <v>10</v>
+      </c>
+      <c r="K48" s="9">
+        <v>10</v>
+      </c>
+      <c r="L48" s="9">
+        <v>10</v>
+      </c>
+      <c r="M48" s="44">
+        <v>10</v>
+      </c>
+      <c r="N48" s="44">
+        <v>10</v>
+      </c>
+      <c r="O48" s="44">
+        <v>10</v>
+      </c>
+      <c r="P48" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q48" s="44">
+        <v>10</v>
+      </c>
+      <c r="R48" s="44">
+        <v>10</v>
+      </c>
+      <c r="S48" s="44">
+        <v>0</v>
+      </c>
+      <c r="T48" s="41"/>
+    </row>
+    <row r="49" spans="1:20" s="2" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B49" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C49" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D46" s="9">
-        <v>10</v>
-      </c>
-      <c r="E46" s="9">
+      <c r="D49" s="9">
+        <v>10</v>
+      </c>
+      <c r="E49" s="9">
         <v>100</v>
       </c>
-      <c r="F46" s="33"/>
-      <c r="G46" s="9">
-        <v>10</v>
-      </c>
-      <c r="H46" s="9">
-        <v>10</v>
-      </c>
-      <c r="I46" s="9">
-        <v>10</v>
-      </c>
-      <c r="J46" s="9">
-        <v>10</v>
-      </c>
-      <c r="K46" s="9">
-        <v>0</v>
-      </c>
-      <c r="L46" s="9">
-        <v>0</v>
-      </c>
-      <c r="M46" s="44">
-        <v>0</v>
-      </c>
-      <c r="N46" s="44">
-        <v>0</v>
-      </c>
-      <c r="O46" s="44">
-        <v>0</v>
-      </c>
-      <c r="P46" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="44">
-        <v>0</v>
-      </c>
-      <c r="R46" s="44">
-        <v>0</v>
-      </c>
-      <c r="S46" s="41"/>
-    </row>
-    <row r="47" spans="1:21" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="10" t="s">
+      <c r="F49" s="33"/>
+      <c r="G49" s="9">
+        <v>10</v>
+      </c>
+      <c r="H49" s="9">
+        <v>10</v>
+      </c>
+      <c r="I49" s="9">
+        <v>10</v>
+      </c>
+      <c r="J49" s="9">
+        <v>10</v>
+      </c>
+      <c r="K49" s="9">
+        <v>10</v>
+      </c>
+      <c r="L49" s="9">
+        <v>10</v>
+      </c>
+      <c r="M49" s="44">
+        <v>10</v>
+      </c>
+      <c r="N49" s="44">
+        <v>10</v>
+      </c>
+      <c r="O49" s="44">
+        <v>10</v>
+      </c>
+      <c r="P49" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q49" s="44">
+        <v>10</v>
+      </c>
+      <c r="R49" s="44">
+        <v>10</v>
+      </c>
+      <c r="S49" s="44">
+        <v>0</v>
+      </c>
+      <c r="T49" s="41"/>
+    </row>
+    <row r="50" spans="1:20" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="20"/>
-      <c r="D47" s="32">
-        <f>SUM(D45:D46)</f>
-        <v>20</v>
-      </c>
-      <c r="E47" s="32">
-        <f>SUM(E45:E46)</f>
-        <v>200</v>
-      </c>
-      <c r="F47" s="36">
+      <c r="C50" s="20"/>
+      <c r="D50" s="32">
+        <f>SUM(D47:D49)</f>
+        <v>30</v>
+      </c>
+      <c r="E50" s="32">
+        <f>SUM(E47:E49)</f>
+        <v>300</v>
+      </c>
+      <c r="F50" s="36">
         <v>-110</v>
       </c>
-      <c r="G47" s="32">
-        <f>SUM(G45:G46)</f>
-        <v>20</v>
-      </c>
-      <c r="H47" s="32">
-        <f>SUM(H45:H46)</f>
-        <v>20</v>
-      </c>
-      <c r="I47" s="32">
-        <f>SUM(I45:I46)</f>
-        <v>20</v>
-      </c>
-      <c r="J47" s="32">
-        <f>SUM(J45:J46)</f>
-        <v>20</v>
-      </c>
-      <c r="K47" s="37">
-        <f>SUM(K45:K46)</f>
-        <v>0</v>
-      </c>
-      <c r="L47" s="37">
-        <f>SUM(S45:S46)</f>
-        <v>0</v>
-      </c>
-      <c r="M47" s="37">
-        <f t="shared" ref="M47:R47" si="2">SUM(T45:T46)</f>
-        <v>0</v>
-      </c>
-      <c r="N47" s="37">
+      <c r="G50" s="32">
+        <f>SUM(G47:G49)</f>
+        <v>30</v>
+      </c>
+      <c r="H50" s="32">
+        <f>SUM(H47:H49)</f>
+        <v>30</v>
+      </c>
+      <c r="I50" s="32">
+        <f>SUM(I47:I49)</f>
+        <v>30</v>
+      </c>
+      <c r="J50" s="32">
+        <f>SUM(J47:J49)</f>
+        <v>30</v>
+      </c>
+      <c r="K50" s="37">
+        <f>SUM(K47:K49)</f>
+        <v>30</v>
+      </c>
+      <c r="L50" s="37">
+        <f>SUM(L47:L49)</f>
+        <v>30</v>
+      </c>
+      <c r="M50" s="37">
+        <f>SUM(M47:M49)</f>
+        <v>30</v>
+      </c>
+      <c r="N50" s="37">
+        <f t="shared" ref="N50:R50" si="2">SUM(N47:N49)</f>
+        <v>30</v>
+      </c>
+      <c r="O50" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O47" s="37">
+        <v>30</v>
+      </c>
+      <c r="P50" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P47" s="37">
+        <v>30</v>
+      </c>
+      <c r="Q50" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q47" s="37">
+        <v>30</v>
+      </c>
+      <c r="R50" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R47" s="37">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S47" s="42">
-        <f>SUM(D47:L47)</f>
-        <v>190</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="23" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
-      <c r="R48" s="22"/>
-    </row>
-    <row r="49" spans="1:18" ht="22" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="22"/>
-      <c r="O49" s="22"/>
-      <c r="P49" s="22"/>
-      <c r="Q49" s="22"/>
-      <c r="R49" s="22"/>
-    </row>
-    <row r="50" spans="1:18" ht="22" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="22"/>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="22"/>
-    </row>
-    <row r="51" spans="1:18" ht="22" x14ac:dyDescent="0.3">
-      <c r="J51" s="35"/>
-      <c r="K51" s="35"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="35"/>
-      <c r="N51" s="35"/>
-      <c r="O51" s="35"/>
-      <c r="P51" s="35"/>
-      <c r="Q51" s="35"/>
-      <c r="R51" s="35"/>
+        <v>30</v>
+      </c>
+      <c r="S50" s="37">
+        <f>SUM(S47:S49)</f>
+        <v>0</v>
+      </c>
+      <c r="T50" s="42">
+        <f>SUM(D50:S50)</f>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" ht="23" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="22"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="22"/>
+      <c r="S51" s="22"/>
+    </row>
+    <row r="52" spans="1:20" ht="22" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="22"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22"/>
+      <c r="P52" s="22"/>
+      <c r="Q52" s="22"/>
+      <c r="R52" s="22"/>
+      <c r="S52" s="22"/>
+    </row>
+    <row r="53" spans="1:20" ht="22" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="22"/>
+      <c r="N53" s="22"/>
+      <c r="O53" s="22"/>
+      <c r="P53" s="22"/>
+      <c r="Q53" s="22"/>
+      <c r="R53" s="22"/>
+      <c r="S53" s="22"/>
+    </row>
+    <row r="54" spans="1:20" ht="22" x14ac:dyDescent="0.3">
+      <c r="J54" s="35"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="35"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="35"/>
+      <c r="P54" s="35"/>
+      <c r="Q54" s="35"/>
+      <c r="R54" s="35"/>
+      <c r="S54" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C46:E46"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>